<commit_message>
fixed scroll on sheets
</commit_message>
<xml_diff>
--- a/applications/template_input.xlsx
+++ b/applications/template_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6E77CBEB-9E4B-044D-85A9-F9E76E974872}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{581F6C99-7ABC-A340-B723-D81E3155E3EE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5597,7 +5597,9 @@
   </sheetPr>
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5978,7 +5980,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6011,85 +6013,45 @@
       <c r="B2" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="76">
-        <f>1.5*0.61</f>
-        <v>0.91500000000000004</v>
-      </c>
-      <c r="D2" s="76">
-        <f>0.5*0.61</f>
-        <v>0.30499999999999999</v>
-      </c>
-      <c r="E2" s="76">
-        <v>0.05</v>
-      </c>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="86"/>
       <c r="B3" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="76">
-        <f>1.5*0.61</f>
-        <v>0.91500000000000004</v>
-      </c>
-      <c r="D3" s="76">
-        <f>0.5*0.61</f>
-        <v>0.30499999999999999</v>
-      </c>
-      <c r="E3" s="76">
-        <v>0.05</v>
-      </c>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="86"/>
       <c r="B4" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="76">
-        <f>1.5*0.61</f>
-        <v>0.91500000000000004</v>
-      </c>
-      <c r="D4" s="76">
-        <f>0.5*0.61</f>
-        <v>0.30499999999999999</v>
-      </c>
-      <c r="E4" s="76">
-        <v>0.05</v>
-      </c>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="86"/>
       <c r="B5" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="76">
-        <f>1.5*0.61</f>
-        <v>0.91500000000000004</v>
-      </c>
-      <c r="D5" s="76">
-        <f>0.5*0.61</f>
-        <v>0.30499999999999999</v>
-      </c>
-      <c r="E5" s="76">
-        <v>0.05</v>
-      </c>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="86"/>
       <c r="B6" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="76">
-        <f>1.5*0.61</f>
-        <v>0.91500000000000004</v>
-      </c>
-      <c r="D6" s="76">
-        <f>0.5*0.61</f>
-        <v>0.30499999999999999</v>
-      </c>
-      <c r="E6" s="76">
-        <v>0.05</v>
-      </c>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" s="85"/>
@@ -6415,7 +6377,7 @@
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -8338,9 +8300,7 @@
   </sheetPr>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9335,9 +9295,7 @@
   </sheetPr>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -10233,9 +10191,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -10337,9 +10293,7 @@
   </sheetPr>
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -10542,9 +10496,7 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -10782,9 +10734,7 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -10844,9 +10794,7 @@
   </sheetPr>
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>

<commit_message>
Removed data from template
</commit_message>
<xml_diff>
--- a/applications/template_input.xlsx
+++ b/applications/template_input.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BA017A47-6BC3-E946-81D2-D4A53A3D86E3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="961" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="11760" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -73,17 +79,17 @@
     <definedName name="term_SGA">'Baseline year population inputs'!$C$47</definedName>
     <definedName name="U5_mortality">'Baseline year population inputs'!$C$39</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="D28" authorId="0">
+    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
       <text>
         <r>
           <rPr>
@@ -109,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D30" authorId="0">
+    <comment ref="D30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000002000000}">
       <text>
         <r>
           <rPr>
@@ -135,7 +141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D37" authorId="0">
+    <comment ref="D37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000003000000}">
       <text>
         <r>
           <rPr>
@@ -166,12 +172,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -195,7 +201,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000002000000}">
       <text>
         <r>
           <rPr>
@@ -224,12 +230,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0F00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -908,7 +914,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -4310,8 +4316,8 @@
     <cellStyle name="Hyperlink" xfId="1445" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1447" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="725"/>
-    <cellStyle name="Normal 3" xfId="726"/>
+    <cellStyle name="Normal 2" xfId="725" xr:uid="{00000000-0005-0000-0000-0000A6050000}"/>
+    <cellStyle name="Normal 3" xfId="726" xr:uid="{00000000-0005-0000-0000-0000A7050000}"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
@@ -4370,7 +4376,7 @@
         <xdr:cNvPr id="2049" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000001080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4427,7 +4433,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4484,7 +4490,7 @@
         <xdr:cNvPr id="3" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4541,7 +4547,7 @@
         <xdr:cNvPr id="4" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4598,7 +4604,7 @@
         <xdr:cNvPr id="5" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4655,7 +4661,7 @@
         <xdr:cNvPr id="6" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4712,7 +4718,7 @@
         <xdr:cNvPr id="7" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4769,7 +4775,7 @@
         <xdr:cNvPr id="8" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4826,7 +4832,7 @@
         <xdr:cNvPr id="9" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4883,7 +4889,7 @@
         <xdr:cNvPr id="10" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4940,7 +4946,7 @@
         <xdr:cNvPr id="11" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4997,7 +5003,7 @@
         <xdr:cNvPr id="12" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5054,7 +5060,7 @@
         <xdr:cNvPr id="13" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5111,7 +5117,7 @@
         <xdr:cNvPr id="14" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5168,7 +5174,7 @@
         <xdr:cNvPr id="15" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5225,7 +5231,7 @@
         <xdr:cNvPr id="16" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5282,7 +5288,7 @@
         <xdr:cNvPr id="17" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5339,7 +5345,7 @@
         <xdr:cNvPr id="18" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5388,7 +5394,7 @@
         <xdr:cNvPr id="19" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5751,24 +5757,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" style="16" customWidth="1"/>
-    <col min="3" max="16384" width="14.42578125" style="12"/>
+    <col min="1" max="1" width="27.6640625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" style="16" customWidth="1"/>
+    <col min="3" max="16384" width="14.5" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
@@ -5779,14 +5785,14 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>193</v>
       </c>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
     </row>
-    <row r="3" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="7" t="s">
         <v>195</v>
@@ -5795,7 +5801,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="9" t="s">
         <v>194</v>
@@ -5804,93 +5810,93 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="16" t="s">
         <v>209</v>
       </c>
       <c r="C7" s="75"/>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="7" t="s">
         <v>106</v>
       </c>
       <c r="C8" s="70"/>
     </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9" t="s">
         <v>107</v>
       </c>
       <c r="C9" s="71"/>
     </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9" t="s">
         <v>105</v>
       </c>
       <c r="C10" s="71"/>
     </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="7" t="s">
         <v>108</v>
       </c>
       <c r="C11" s="70"/>
     </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="7" t="s">
         <v>109</v>
       </c>
       <c r="C12" s="70"/>
     </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="7" t="s">
         <v>110</v>
       </c>
       <c r="C13" s="70"/>
     </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12"/>
     </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="12" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="9" t="s">
         <v>94</v>
       </c>
       <c r="C16" s="71"/>
     </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="9" t="s">
         <v>95</v>
       </c>
       <c r="C17" s="71"/>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="9" t="s">
         <v>96</v>
       </c>
       <c r="C18" s="71"/>
     </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="9" t="s">
         <v>97</v>
       </c>
       <c r="C19" s="71"/>
     </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="9" t="s">
         <v>98</v>
       </c>
@@ -5899,74 +5905,74 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="12"/>
     </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="20" t="s">
         <v>101</v>
       </c>
       <c r="C23" s="71"/>
     </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="20" t="s">
         <v>102</v>
       </c>
       <c r="C24" s="71"/>
     </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="20" t="s">
         <v>103</v>
       </c>
       <c r="C25" s="71"/>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="20" t="s">
         <v>104</v>
       </c>
       <c r="C26" s="71"/>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
     </row>
-    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
         <v>200</v>
       </c>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
     </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="30" t="s">
         <v>75</v>
       </c>
       <c r="C29" s="73"/>
     </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="30" t="s">
         <v>76</v>
       </c>
       <c r="C30" s="73"/>
     </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="30" t="s">
         <v>77</v>
       </c>
       <c r="C31" s="73"/>
     </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="30" t="s">
         <v>78</v>
       </c>
       <c r="C32" s="73"/>
     </row>
-    <row r="33" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="B33" s="32" t="s">
         <v>129</v>
       </c>
@@ -5975,26 +5981,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="12" t="s">
         <v>74</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="13"/>
     </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="42" t="s">
         <v>92</v>
       </c>
       <c r="C37" s="72"/>
     </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="16" t="s">
         <v>91</v>
       </c>
@@ -6002,7 +6008,7 @@
       <c r="D38" s="17"/>
       <c r="E38" s="18"/>
     </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="16" t="s">
         <v>90</v>
       </c>
@@ -6010,48 +6016,48 @@
       <c r="D39" s="17"/>
       <c r="E39" s="17"/>
     </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="16" t="s">
         <v>171</v>
       </c>
       <c r="C40" s="72"/>
     </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="16" t="s">
         <v>89</v>
       </c>
       <c r="C41" s="71"/>
     </row>
-    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="42" t="s">
         <v>93</v>
       </c>
       <c r="C42" s="72"/>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D43" s="17"/>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="12" t="s">
         <v>133</v>
       </c>
       <c r="D44" s="17"/>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C45" s="71"/>
       <c r="D45" s="17"/>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C46" s="71"/>
       <c r="D46" s="17"/>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="16" t="s">
         <v>12</v>
       </c>
@@ -6059,7 +6065,7 @@
       <c r="D47" s="17"/>
       <c r="E47" s="18"/>
     </row>
-    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="16" t="s">
         <v>26</v>
       </c>
@@ -6070,52 +6076,52 @@
       <c r="D48" s="17"/>
       <c r="E48" s="17"/>
     </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D49" s="17"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="12" t="s">
         <v>72</v>
       </c>
       <c r="D50" s="17"/>
     </row>
-    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B51" s="16" t="s">
         <v>124</v>
       </c>
       <c r="C51" s="69"/>
       <c r="D51" s="17"/>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B52" s="16" t="s">
         <v>125</v>
       </c>
       <c r="C52" s="69"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B53" s="16" t="s">
         <v>126</v>
       </c>
       <c r="C53" s="69"/>
     </row>
-    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B54" s="16" t="s">
         <v>127</v>
       </c>
       <c r="C54" s="69"/>
     </row>
-    <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B55" s="16" t="s">
         <v>128</v>
       </c>
       <c r="C55" s="69"/>
     </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="12" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B58" s="7" t="s">
         <v>111</v>
       </c>
@@ -6123,13 +6129,13 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B59" s="16" t="s">
         <v>132</v>
       </c>
       <c r="C59" s="70"/>
     </row>
-    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="4"/>
     </row>
   </sheetData>
@@ -6143,7 +6149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -6153,13 +6159,13 @@
       <selection activeCell="C2" sqref="C2:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="56" customWidth="1"/>
-    <col min="2" max="16384" width="10.85546875" style="56"/>
+    <col min="1" max="1" width="18.6640625" style="56" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="40" x14ac:dyDescent="0.2">
       <c r="A1" s="61" t="s">
         <v>196</v>
       </c>
@@ -6176,7 +6182,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="59" t="s">
         <v>164</v>
       </c>
@@ -6187,7 +6193,7 @@
       <c r="D2" s="90"/>
       <c r="E2" s="90"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="58"/>
       <c r="B3" s="58" t="s">
         <v>1</v>
@@ -6196,7 +6202,7 @@
       <c r="D3" s="90"/>
       <c r="E3" s="90"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="58"/>
       <c r="B4" s="58" t="s">
         <v>2</v>
@@ -6205,7 +6211,7 @@
       <c r="D4" s="90"/>
       <c r="E4" s="90"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="58"/>
       <c r="B5" s="58" t="s">
         <v>3</v>
@@ -6214,7 +6220,7 @@
       <c r="D5" s="90"/>
       <c r="E5" s="90"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="58"/>
       <c r="B6" s="58" t="s">
         <v>4</v>
@@ -6223,7 +6229,7 @@
       <c r="D6" s="90"/>
       <c r="E6" s="90"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" s="57"/>
     </row>
   </sheetData>
@@ -6233,7 +6239,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -6243,15 +6249,15 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="53" style="53" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.85546875" style="35" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" style="35" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="35"/>
+    <col min="2" max="2" width="47.83203125" style="35" customWidth="1"/>
+    <col min="3" max="3" width="42.5" style="35" customWidth="1"/>
+    <col min="4" max="16384" width="11.5" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="40" t="s">
         <v>69</v>
       </c>
@@ -6262,7 +6268,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="93" t="s">
         <v>189</v>
       </c>
@@ -6271,7 +6277,7 @@
       </c>
       <c r="C2" s="85"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="93" t="s">
         <v>207</v>
       </c>
@@ -6280,7 +6286,7 @@
       </c>
       <c r="C3" s="85"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="94" t="s">
         <v>58</v>
       </c>
@@ -6289,7 +6295,7 @@
       </c>
       <c r="C4" s="85"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="94" t="s">
         <v>137</v>
       </c>
@@ -6298,104 +6304,104 @@
       </c>
       <c r="C5" s="85"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="94"/>
       <c r="B6" s="92"/>
       <c r="C6" s="92"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="94"/>
       <c r="B7" s="92"/>
       <c r="C7" s="92"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="94"/>
       <c r="B8" s="92"/>
       <c r="C8" s="92"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="94"/>
       <c r="B9" s="92"/>
       <c r="C9" s="92"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="94"/>
       <c r="B10" s="92"/>
       <c r="C10" s="92"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="95"/>
       <c r="B11" s="92"/>
       <c r="C11" s="92"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="95"/>
       <c r="B12" s="92"/>
       <c r="C12" s="92"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="95"/>
       <c r="B13" s="92"/>
       <c r="C13" s="92"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="95"/>
       <c r="B14" s="92"/>
       <c r="C14" s="92"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="95"/>
       <c r="B15" s="92"/>
       <c r="C15" s="92"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="95"/>
       <c r="B16" s="92"/>
       <c r="C16" s="92"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="95"/>
       <c r="B17" s="92"/>
       <c r="C17" s="92"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="95"/>
       <c r="B18" s="92"/>
       <c r="C18" s="92"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="94"/>
       <c r="B19" s="92"/>
       <c r="C19" s="92"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="94"/>
       <c r="B20" s="92"/>
       <c r="C20" s="92"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="94"/>
       <c r="B21" s="92"/>
       <c r="C21" s="92"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="94"/>
       <c r="B22" s="92"/>
       <c r="C22" s="92"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B23" s="92"/>
       <c r="C23" s="92"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B24" s="92"/>
       <c r="C24" s="92"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B25" s="92"/>
       <c r="C25" s="92"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B26" s="92"/>
       <c r="C26" s="92"/>
     </row>
@@ -6408,7 +6414,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -6418,85 +6424,85 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="30.140625" style="35" customWidth="1"/>
-    <col min="2" max="16384" width="11.42578125" style="35"/>
+    <col min="1" max="1" width="30.1640625" style="35" customWidth="1"/>
+    <col min="2" max="16384" width="11.5" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="40" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="48" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" s="48" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" s="48" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" s="48" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" s="48" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" s="48" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" s="48" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" s="48" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" s="48"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" s="48"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" s="48"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" s="48"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A14" s="48"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" s="48"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" s="48"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="48"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="48"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" s="48"/>
     </row>
   </sheetData>
@@ -6506,7 +6512,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
   </sheetPr>
@@ -6516,9 +6522,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -6538,7 +6544,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>71</v>
       </c>
@@ -6563,7 +6569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>65</v>
       </c>
@@ -6588,7 +6594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>66</v>
       </c>
@@ -6620,7 +6626,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -6630,19 +6636,19 @@
       <selection activeCell="C29" activeCellId="3" sqref="C2:O12 C14:O21 C23:O27 C29:O38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -6689,7 +6695,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
@@ -6740,7 +6746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="7" t="s">
         <v>149</v>
       </c>
@@ -6784,7 +6790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="7" t="s">
         <v>197</v>
       </c>
@@ -6828,7 +6834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="11" t="s">
         <v>136</v>
       </c>
@@ -6874,7 +6880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="11" t="s">
         <v>137</v>
       </c>
@@ -6921,7 +6927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="33" t="s">
         <v>84</v>
       </c>
@@ -6970,7 +6976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="11" t="s">
         <v>58</v>
       </c>
@@ -7016,7 +7022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="11" t="s">
         <v>67</v>
       </c>
@@ -7064,7 +7070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="11" t="s">
         <v>28</v>
       </c>
@@ -7108,7 +7114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="33" t="s">
         <v>85</v>
       </c>
@@ -7157,7 +7163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="11" t="s">
         <v>60</v>
       </c>
@@ -7201,10 +7207,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="33"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -7255,7 +7261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="11" t="s">
         <v>86</v>
@@ -7300,7 +7306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="11" t="s">
         <v>189</v>
@@ -7349,7 +7355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="11" t="s">
         <v>207</v>
@@ -7398,7 +7404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="33" t="s">
         <v>57</v>
       </c>
@@ -7446,7 +7452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="11" t="s">
         <v>88</v>
       </c>
@@ -7490,7 +7496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="11" t="s">
         <v>87</v>
       </c>
@@ -7534,7 +7540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="33" t="s">
         <v>59</v>
       </c>
@@ -7582,10 +7588,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="33"/>
     </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="64" t="s">
         <v>37</v>
       </c>
@@ -7636,7 +7642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="65" t="s">
         <v>190</v>
       </c>
@@ -7684,7 +7690,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="65" t="s">
         <v>208</v>
       </c>
@@ -7732,7 +7738,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="65" t="s">
         <v>191</v>
       </c>
@@ -7780,7 +7786,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="65" t="s">
         <v>192</v>
       </c>
@@ -7825,7 +7831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="11"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -7835,7 +7841,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
@@ -7893,7 +7899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="11" t="s">
         <v>64</v>
       </c>
@@ -7948,7 +7954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="11" t="s">
         <v>62</v>
       </c>
@@ -8003,7 +8009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="11" t="s">
         <v>47</v>
       </c>
@@ -8047,7 +8053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="11" t="s">
         <v>34</v>
       </c>
@@ -8104,7 +8110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="33" t="s">
         <v>83</v>
       </c>
@@ -8148,7 +8154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="5"/>
       <c r="B35" s="33" t="s">
         <v>82</v>
@@ -8193,7 +8199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="33" t="s">
         <v>81</v>
       </c>
@@ -8237,7 +8243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="33" t="s">
         <v>79</v>
       </c>
@@ -8281,7 +8287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="33" t="s">
         <v>80</v>
       </c>
@@ -8325,7 +8331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="33"/>
     </row>
   </sheetData>
@@ -8339,31 +8345,31 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" s="12" t="s">
         <v>205</v>
       </c>
@@ -8374,7 +8380,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -8384,16 +8390,16 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" style="35" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="35" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" style="35"/>
-    <col min="5" max="5" width="17.42578125" style="35" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="35"/>
+    <col min="1" max="1" width="33.6640625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="35" customWidth="1"/>
+    <col min="3" max="4" width="11.5" style="35"/>
+    <col min="5" max="5" width="17.5" style="35" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="40" t="s">
         <v>163</v>
       </c>
@@ -8410,7 +8416,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="39" t="s">
         <v>158</v>
       </c>
@@ -8428,7 +8434,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="39" t="s">
         <v>157</v>
       </c>
@@ -8446,7 +8452,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="39" t="s">
         <v>156</v>
       </c>
@@ -8464,7 +8470,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="39" t="s">
         <v>155</v>
       </c>
@@ -8482,7 +8488,7 @@
         <v>0.126</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="39" t="s">
         <v>154</v>
       </c>
@@ -8500,7 +8506,7 @@
         <v>1.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="39" t="s">
         <v>153</v>
       </c>
@@ -8518,7 +8524,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="39" t="s">
         <v>152</v>
       </c>
@@ -8536,7 +8542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="39" t="s">
         <v>151</v>
       </c>
@@ -8554,7 +8560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="39" t="s">
         <v>150</v>
       </c>
@@ -8572,7 +8578,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C11" s="36"/>
     </row>
   </sheetData>
@@ -8583,7 +8589,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -8593,14 +8599,14 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="12" customWidth="1"/>
-    <col min="2" max="9" width="16.85546875" style="12" customWidth="1"/>
-    <col min="10" max="16384" width="14.42578125" style="12"/>
+    <col min="1" max="1" width="8.5" style="12" customWidth="1"/>
+    <col min="2" max="9" width="16.83203125" style="12" customWidth="1"/>
+    <col min="10" max="16384" width="14.5" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -8629,7 +8635,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="97">
         <f>start_year</f>
         <v>2017</v>
@@ -8652,7 +8658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="97">
         <f t="shared" ref="A3:A40" si="2">IF($A$2+ROW(A3)-2&lt;=end_year,A2+1,"")</f>
         <v>2018</v>
@@ -8675,7 +8681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="97">
         <f t="shared" si="2"/>
         <v>2019</v>
@@ -8698,7 +8704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="97">
         <f t="shared" si="2"/>
         <v>2020</v>
@@ -8721,7 +8727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="97">
         <f t="shared" si="2"/>
         <v>2021</v>
@@ -8744,7 +8750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="97">
         <f t="shared" si="2"/>
         <v>2022</v>
@@ -8767,7 +8773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="97">
         <f t="shared" si="2"/>
         <v>2023</v>
@@ -8790,7 +8796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="97">
         <f t="shared" si="2"/>
         <v>2024</v>
@@ -8813,7 +8819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="97">
         <f t="shared" si="2"/>
         <v>2025</v>
@@ -8836,7 +8842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="97">
         <f t="shared" si="2"/>
         <v>2026</v>
@@ -8859,7 +8865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="97">
         <f t="shared" si="2"/>
         <v>2027</v>
@@ -8882,7 +8888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="97">
         <f t="shared" si="2"/>
         <v>2028</v>
@@ -8905,7 +8911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="97">
         <f t="shared" si="2"/>
         <v>2029</v>
@@ -8928,7 +8934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="97">
         <f t="shared" si="2"/>
         <v>2030</v>
@@ -8951,7 +8957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8974,7 +8980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -8997,7 +9003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9020,7 +9026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9043,7 +9049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9066,7 +9072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9089,7 +9095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9112,7 +9118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9135,7 +9141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9158,7 +9164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9181,7 +9187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9204,7 +9210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9227,7 +9233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9250,7 +9256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9273,7 +9279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9296,7 +9302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9319,7 +9325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9342,7 +9348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9365,7 +9371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9388,7 +9394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9411,7 +9417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9434,7 +9440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9457,7 +9463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9480,7 +9486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9503,7 +9509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="97" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -9539,24 +9545,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
     <col min="3" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="str">
         <f>"Percentage of deaths in baseline year ("&amp;start_year&amp;") attributable to cause"</f>
         <v>Percentage of deaths in baseline year (2017) attributable to cause</v>
@@ -9567,7 +9573,7 @@
       <c r="E1" s="41"/>
       <c r="F1" s="41"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>210</v>
       </c>
@@ -9582,82 +9588,66 @@
       <c r="F2" s="41"/>
       <c r="G2" s="41"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="80">
-        <v>2.7000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="80"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="80">
-        <v>0.1966</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="80"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="80">
-        <v>6.2100000000000002E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="80"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="80">
-        <v>0.29289999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="80"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="80">
-        <v>0.24709999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="80"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="80">
-        <v>4.7999999999999996E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="80"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="80">
-        <v>0.13200000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="80"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="80">
-        <v>6.1800000000000001E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="80"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="32" t="s">
         <v>129</v>
       </c>
       <c r="C11" s="96">
         <f>SUM(C3:C10)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="32"/>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
@@ -9666,7 +9656,7 @@
       <c r="G12" s="24"/>
       <c r="H12" s="24"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
         <v>31</v>
       </c>
@@ -9687,183 +9677,111 @@
       </c>
       <c r="G13" s="24"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="80">
-        <v>0.1368</v>
-      </c>
-      <c r="D14" s="80">
-        <v>0.1368</v>
-      </c>
-      <c r="E14" s="80">
-        <v>0.1368</v>
-      </c>
-      <c r="F14" s="80">
-        <v>0.1368</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="80">
-        <v>0.20660000000000001</v>
-      </c>
-      <c r="D15" s="80">
-        <v>0.20660000000000001</v>
-      </c>
-      <c r="E15" s="80">
-        <v>0.20660000000000001</v>
-      </c>
-      <c r="F15" s="80">
-        <v>0.20660000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="80">
-        <v>2.1100000000000001E-2</v>
-      </c>
-      <c r="D16" s="80">
-        <v>2.1100000000000001E-2</v>
-      </c>
-      <c r="E16" s="80">
-        <v>2.1100000000000001E-2</v>
-      </c>
-      <c r="F16" s="80">
-        <v>2.1100000000000001E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="80">
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="D17" s="80">
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="E17" s="80">
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="F17" s="80">
-        <v>7.4999999999999997E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="80"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="80"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="80">
-        <v>8.6199999999999999E-2</v>
-      </c>
-      <c r="D18" s="80">
-        <v>8.6199999999999999E-2</v>
-      </c>
-      <c r="E18" s="80">
-        <v>8.6199999999999999E-2</v>
-      </c>
-      <c r="F18" s="80">
-        <v>8.6199999999999999E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="80"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="80"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="80">
-        <v>2.86E-2</v>
-      </c>
-      <c r="D19" s="80">
-        <v>2.86E-2</v>
-      </c>
-      <c r="E19" s="80">
-        <v>2.86E-2</v>
-      </c>
-      <c r="F19" s="80">
-        <v>2.86E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="80"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="80">
-        <v>1.5299999999999999E-2</v>
-      </c>
-      <c r="D20" s="80">
-        <v>1.5299999999999999E-2</v>
-      </c>
-      <c r="E20" s="80">
-        <v>1.5299999999999999E-2</v>
-      </c>
-      <c r="F20" s="80">
-        <v>1.5299999999999999E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="80"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="80">
-        <v>0.13589999999999999</v>
-      </c>
-      <c r="D21" s="80">
-        <v>0.13589999999999999</v>
-      </c>
-      <c r="E21" s="80">
-        <v>0.13589999999999999</v>
-      </c>
-      <c r="F21" s="80">
-        <v>0.13589999999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="80"/>
+      <c r="D21" s="80"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="80"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="80">
-        <v>0.36199999999999999</v>
-      </c>
-      <c r="D22" s="80">
-        <v>0.36199999999999999</v>
-      </c>
-      <c r="E22" s="80">
-        <v>0.36199999999999999</v>
-      </c>
-      <c r="F22" s="80">
-        <v>0.36199999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="32" t="s">
         <v>129</v>
       </c>
       <c r="C23" s="96">
         <f>SUM(C14:C22)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="96">
-        <f t="shared" ref="D23:F23" si="0">SUM(D14:D22)</f>
-        <v>1</v>
+        <f t="shared" ref="D23:E23" si="0">SUM(D14:D22)</f>
+        <v>0</v>
       </c>
       <c r="E23" s="96">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" s="96">
         <f>SUM(F14:F22)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" s="24"/>
       <c r="H23" s="24"/>
     </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="32"/>
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
@@ -9872,7 +9790,7 @@
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -9888,85 +9806,67 @@
       <c r="G25" s="24"/>
       <c r="H25" s="24"/>
     </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="80">
-        <v>0.10082724000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="80"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="80">
-        <v>3.1206000000000002E-4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C27" s="80"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="80">
-        <v>0.15891214000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="80"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="80">
-        <v>0.12598688999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C29" s="80"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="80">
-        <v>0.12434007</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C30" s="80"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="80">
-        <v>3.9028409999999999E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="80"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="80">
-        <v>8.5254999999999999E-4</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C32" s="80"/>
+    </row>
+    <row r="33" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="80">
-        <v>6.8467810000000004E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="80"/>
+    </row>
+    <row r="34" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="80">
-        <v>0.38127283000000001</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="80"/>
+    </row>
+    <row r="35" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" s="32" t="s">
         <v>129</v>
       </c>
       <c r="C35" s="96">
         <f>SUM(C26:C34)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -9978,7 +9878,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -9988,13 +9888,13 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.5" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="27" t="str">
         <f>"Percentage of population in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of population in each category in baseline year (2017)</v>
@@ -10018,7 +9918,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>115</v>
       </c>
@@ -10046,33 +9946,33 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5"/>
       <c r="B3" s="11" t="s">
         <v>118</v>
       </c>
       <c r="C3" s="81" t="str">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C4:C5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - SUM(C4:C5), "")</f>
         <v/>
       </c>
       <c r="D3" s="81" t="str">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D4:D5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - SUM(D4:D5), "")</f>
         <v/>
       </c>
       <c r="E3" s="81" t="str">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(E4:E5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - SUM(E4:E5), "")</f>
         <v/>
       </c>
       <c r="F3" s="81" t="str">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(F4:F5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - SUM(F4:F5), "")</f>
         <v/>
       </c>
       <c r="G3" s="81" t="str">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(G4:G5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - SUM(G4:G5), "")</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
       <c r="B4" s="11" t="s">
         <v>116</v>
@@ -10083,7 +9983,7 @@
       <c r="F4" s="82"/>
       <c r="G4" s="82"/>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5"/>
       <c r="B5" s="11" t="s">
         <v>119</v>
@@ -10094,7 +9994,7 @@
       <c r="F5" s="82"/>
       <c r="G5" s="82"/>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="14"/>
       <c r="C6" s="29"/>
       <c r="D6" s="29"/>
@@ -10102,7 +10002,7 @@
       <c r="F6" s="29"/>
       <c r="G6" s="29"/>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="14"/>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -10110,7 +10010,7 @@
       <c r="F7" s="29"/>
       <c r="G7" s="29"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>114</v>
       </c>
@@ -10138,32 +10038,32 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="7" t="s">
         <v>121</v>
       </c>
       <c r="C9" s="81" t="str">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C10:C11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - SUM(C10:C11), "")</f>
         <v/>
       </c>
       <c r="D9" s="81" t="str">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D10:D11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - SUM(D10:D11), "")</f>
         <v/>
       </c>
       <c r="E9" s="81" t="str">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(E10:E11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - SUM(E10:E11), "")</f>
         <v/>
       </c>
       <c r="F9" s="81" t="str">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(F10:F11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - SUM(F10:F11), "")</f>
         <v/>
       </c>
       <c r="G9" s="81" t="str">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(G10:G11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - SUM(G10:G11), "")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="7" t="s">
         <v>122</v>
       </c>
@@ -10173,7 +10073,7 @@
       <c r="F10" s="82"/>
       <c r="G10" s="82"/>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="7" t="s">
         <v>123</v>
       </c>
@@ -10183,7 +10083,7 @@
       <c r="F11" s="82"/>
       <c r="G11" s="82"/>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -10197,7 +10097,7 @@
       <c r="N12" s="15"/>
       <c r="O12" s="15"/>
     </row>
-    <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
         <v>70</v>
       </c>
@@ -10241,7 +10141,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="16" t="s">
         <v>131</v>
       </c>
@@ -10259,7 +10159,7 @@
       <c r="N14" s="84"/>
       <c r="O14" s="84"/>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="16" t="s">
         <v>68</v>
       </c>
@@ -10316,14 +10216,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -10339,7 +10239,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -10349,13 +10249,13 @@
       <selection activeCell="C2" sqref="C2:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="7" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="2" max="7" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="27" t="str">
         <f>"Percentage of children in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of children in each category in baseline year (2017)</v>
@@ -10379,7 +10279,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -10392,7 +10292,7 @@
       <c r="F2" s="82"/>
       <c r="G2" s="82"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B3" s="43" t="s">
         <v>167</v>
       </c>
@@ -10402,7 +10302,7 @@
       <c r="F3" s="82"/>
       <c r="G3" s="82"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B4" s="43" t="s">
         <v>168</v>
       </c>
@@ -10412,7 +10312,7 @@
       <c r="F4" s="82"/>
       <c r="G4" s="82"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B5" s="43" t="s">
         <v>169</v>
       </c>
@@ -10444,7 +10344,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -10452,13 +10352,13 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>138</v>
       </c>
@@ -10493,7 +10393,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>139</v>
       </c>
@@ -10510,10 +10410,10 @@
       <c r="J2" s="28"/>
       <c r="K2" s="28"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B3" s="14"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -10530,10 +10430,10 @@
       <c r="J4" s="28"/>
       <c r="K4" s="28"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B5" s="14"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -10550,7 +10450,7 @@
       <c r="J6" s="28"/>
       <c r="K6" s="28"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B7" s="14" t="s">
         <v>32</v>
       </c>
@@ -10564,7 +10464,7 @@
       <c r="J7" s="28"/>
       <c r="K7" s="28"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B8" s="14" t="s">
         <v>144</v>
       </c>
@@ -10578,7 +10478,7 @@
       <c r="J8" s="28"/>
       <c r="K8" s="28"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>142</v>
       </c>
@@ -10595,7 +10495,7 @@
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B11" s="34" t="s">
         <v>146</v>
       </c>
@@ -10609,7 +10509,7 @@
       <c r="J11" s="28"/>
       <c r="K11" s="28"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
         <v>74</v>
       </c>
@@ -10626,7 +10526,7 @@
       <c r="J13" s="28"/>
       <c r="K13" s="28"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B14" s="16" t="s">
         <v>170</v>
       </c>
@@ -10647,7 +10547,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -10657,15 +10557,15 @@
       <selection activeCell="E21" activeCellId="5" sqref="C2:D6 E7 C9:D13 E14 C16:D20 E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17" style="35" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="35" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="35"/>
+    <col min="2" max="2" width="19.1640625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="35" customWidth="1"/>
+    <col min="4" max="16384" width="11.5" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="51" t="s">
         <v>180</v>
       </c>
@@ -10682,7 +10582,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="49" t="s">
         <v>175</v>
       </c>
@@ -10696,7 +10596,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="47"/>
       <c r="B3" s="46" t="s">
         <v>1</v>
@@ -10708,7 +10608,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="47"/>
       <c r="B4" s="46" t="s">
         <v>2</v>
@@ -10720,7 +10620,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="47"/>
       <c r="B5" s="46" t="s">
         <v>3</v>
@@ -10732,7 +10632,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="47"/>
       <c r="B6" s="46" t="s">
         <v>4</v>
@@ -10744,7 +10644,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="47"/>
       <c r="B7" s="46" t="s">
         <v>172</v>
@@ -10753,7 +10653,7 @@
       <c r="D7" s="44"/>
       <c r="E7" s="85"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="51" t="s">
         <v>174</v>
       </c>
@@ -10764,7 +10664,7 @@
       <c r="D9" s="85"/>
       <c r="E9" s="63"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="47"/>
       <c r="B10" s="46" t="s">
         <v>1</v>
@@ -10773,7 +10673,7 @@
       <c r="D10" s="85"/>
       <c r="E10" s="62"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="47"/>
       <c r="B11" s="46" t="s">
         <v>2</v>
@@ -10782,7 +10682,7 @@
       <c r="D11" s="85"/>
       <c r="E11" s="62"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="47"/>
       <c r="B12" s="46" t="s">
         <v>3</v>
@@ -10791,7 +10691,7 @@
       <c r="D12" s="85"/>
       <c r="E12" s="62"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="47"/>
       <c r="B13" s="46" t="s">
         <v>4</v>
@@ -10800,7 +10700,7 @@
       <c r="D13" s="85"/>
       <c r="E13" s="62"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="47"/>
       <c r="B14" s="46" t="s">
         <v>172</v>
@@ -10809,7 +10709,7 @@
       <c r="D14" s="44"/>
       <c r="E14" s="85"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="49" t="s">
         <v>173</v>
       </c>
@@ -10823,7 +10723,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="47"/>
       <c r="B17" s="46" t="s">
         <v>1</v>
@@ -10835,7 +10735,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="47"/>
       <c r="B18" s="46" t="s">
         <v>2</v>
@@ -10847,7 +10747,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="47"/>
       <c r="B19" s="46" t="s">
         <v>3</v>
@@ -10859,7 +10759,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="47"/>
       <c r="B20" s="46" t="s">
         <v>4</v>
@@ -10871,7 +10771,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="47"/>
       <c r="B21" s="46" t="s">
         <v>172</v>
@@ -10888,7 +10788,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -10898,15 +10798,15 @@
       <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="66" t="s">
         <v>164</v>
       </c>
@@ -10920,7 +10820,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="67" t="s">
         <v>69</v>
       </c>
@@ -10932,7 +10832,7 @@
       </c>
       <c r="D2" s="85"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="67" t="s">
         <v>187</v>
       </c>
@@ -10951,7 +10851,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -10961,17 +10861,17 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="56" style="53" customWidth="1"/>
     <col min="2" max="2" width="20" style="36" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="35" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="35" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="14.42578125" style="35"/>
+    <col min="3" max="3" width="20.5" style="35" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" style="35" customWidth="1"/>
+    <col min="5" max="5" width="32.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="55" t="s">
         <v>69</v>
       </c>
@@ -10989,7 +10889,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="53" t="s">
         <v>29</v>
       </c>
@@ -11006,7 +10906,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="53" t="s">
         <v>86</v>
       </c>
@@ -11023,7 +10923,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="53" t="s">
         <v>61</v>
       </c>
@@ -11040,7 +10940,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="53" t="s">
         <v>149</v>
       </c>
@@ -11057,7 +10957,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="53" t="s">
         <v>198</v>
       </c>
@@ -11074,7 +10974,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="53" t="s">
         <v>63</v>
       </c>
@@ -11091,7 +10991,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="53" t="s">
         <v>64</v>
       </c>
@@ -11108,7 +11008,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="53" t="s">
         <v>62</v>
       </c>
@@ -11125,7 +11025,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="65" t="s">
         <v>190</v>
       </c>
@@ -11142,7 +11042,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="65" t="s">
         <v>208</v>
       </c>
@@ -11159,7 +11059,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="65" t="s">
         <v>191</v>
       </c>
@@ -11176,7 +11076,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="65" t="s">
         <v>192</v>
       </c>
@@ -11193,7 +11093,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="11" t="s">
         <v>189</v>
       </c>
@@ -11210,7 +11110,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="11" t="s">
         <v>207</v>
       </c>
@@ -11227,7 +11127,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="53" t="s">
         <v>57</v>
       </c>
@@ -11244,7 +11144,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="53" t="s">
         <v>47</v>
       </c>
@@ -11261,7 +11161,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="53" t="s">
         <v>175</v>
       </c>
@@ -11279,7 +11179,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="53" t="s">
         <v>174</v>
       </c>
@@ -11297,7 +11197,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="53" t="s">
         <v>173</v>
       </c>
@@ -11315,7 +11215,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="53" t="s">
         <v>197</v>
       </c>
@@ -11332,7 +11232,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="53" t="s">
         <v>136</v>
       </c>
@@ -11349,7 +11249,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="53" t="s">
         <v>34</v>
       </c>
@@ -11366,7 +11266,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="53" t="s">
         <v>88</v>
       </c>
@@ -11383,7 +11283,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="53" t="s">
         <v>87</v>
       </c>
@@ -11400,7 +11300,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="53" t="s">
         <v>137</v>
       </c>
@@ -11417,7 +11317,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="53" t="s">
         <v>59</v>
       </c>
@@ -11434,7 +11334,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="53" t="s">
         <v>84</v>
       </c>
@@ -11451,7 +11351,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="53" t="s">
         <v>58</v>
       </c>
@@ -11468,7 +11368,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="53" t="s">
         <v>67</v>
       </c>
@@ -11485,7 +11385,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="53" t="s">
         <v>28</v>
       </c>
@@ -11502,7 +11402,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="53" t="s">
         <v>83</v>
       </c>
@@ -11519,7 +11419,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="53" t="s">
         <v>82</v>
       </c>
@@ -11536,7 +11436,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="53" t="s">
         <v>81</v>
       </c>
@@ -11553,7 +11453,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="53" t="s">
         <v>79</v>
       </c>
@@ -11570,7 +11470,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="53" t="s">
         <v>80</v>
       </c>
@@ -11588,7 +11488,7 @@
       </c>
       <c r="F36" s="35"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="53" t="s">
         <v>85</v>
       </c>
@@ -11605,7 +11505,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="53" t="s">
         <v>60</v>
       </c>
@@ -11622,7 +11522,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F39" s="36"/>
     </row>
   </sheetData>
@@ -11636,7 +11536,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000000000000}">
           <x14:formula1>
             <xm:f>'Cost curve options'!$A$1:$A$4</xm:f>
           </x14:formula1>

</xml_diff>